<commit_message>
Fixes and more saves + Oopen Stage controll update
Did A lot off offline work, Fixed some issues upgraded the Interface to the new Open Stage Control. OlimexGateway did not work. Added more config slots.
</commit_message>
<xml_diff>
--- a/extras/OpenStageControl/timecalc.xlsx
+++ b/extras/OpenStageControl/timecalc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\TinyPixelMapper\extras\OpenStageControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA7888B-781F-4101-835B-DA37DBDC40C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D03D8E1-319F-4E5A-8EF2-A16A194E8C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="7793" windowWidth="10395" windowHeight="1230" activeTab="2" xr2:uid="{972FB674-5469-4EBD-9442-7C5F8A1D6208}"/>
+    <workbookView xWindow="-8" yWindow="6353" windowWidth="21601" windowHeight="11422" activeTab="2" xr2:uid="{972FB674-5469-4EBD-9442-7C5F8A1D6208}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -704,10 +704,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C860BA16-8038-4316-8DD0-F6F55D6D66FD}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -725,16 +725,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>4095/A2</f>
-        <v>4095</v>
+        <f>A16/A2</f>
+        <v>4096</v>
       </c>
       <c r="C2">
         <f>B2/2</f>
-        <v>2047.5</v>
+        <v>2048</v>
       </c>
       <c r="D2">
         <f>B2*2</f>
-        <v>8190</v>
+        <v>8192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -742,16 +742,16 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B11" si="0">4095/A3</f>
-        <v>511.875</v>
+        <f>A16/A3</f>
+        <v>512</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C11" si="1">B3/2</f>
-        <v>255.9375</v>
+        <f t="shared" ref="C3:C11" si="0">B3/2</f>
+        <v>256</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="2">B3*2</f>
-        <v>1023.75</v>
+        <f t="shared" ref="D3:D11" si="1">B3*2</f>
+        <v>1024</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
@@ -759,16 +759,16 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>341.25</v>
+        <f>A16/A4</f>
+        <v>341.33333333333331</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
-        <v>170.625</v>
+        <f t="shared" si="0"/>
+        <v>170.66666666666666</v>
       </c>
       <c r="D4">
-        <f t="shared" si="2"/>
-        <v>682.5</v>
+        <f t="shared" si="1"/>
+        <v>682.66666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -776,16 +776,16 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>255.9375</v>
+        <f>A16/A5</f>
+        <v>256</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
-        <v>127.96875</v>
+        <f t="shared" si="0"/>
+        <v>128</v>
       </c>
       <c r="D5">
-        <f t="shared" si="2"/>
-        <v>511.875</v>
+        <f t="shared" si="1"/>
+        <v>512</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
@@ -793,16 +793,16 @@
         <v>24</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>170.625</v>
+        <f>A16/A6</f>
+        <v>170.66666666666666</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
-        <v>85.3125</v>
+        <f t="shared" si="0"/>
+        <v>85.333333333333329</v>
       </c>
       <c r="D6">
-        <f t="shared" si="2"/>
-        <v>341.25</v>
+        <f t="shared" si="1"/>
+        <v>341.33333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
@@ -810,16 +810,16 @@
         <v>32</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>127.96875</v>
+        <f>A16/A7</f>
+        <v>128</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
-        <v>63.984375</v>
+        <f t="shared" si="0"/>
+        <v>64</v>
       </c>
       <c r="D7">
-        <f t="shared" si="2"/>
-        <v>255.9375</v>
+        <f t="shared" si="1"/>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -827,16 +827,16 @@
         <v>40</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>102.375</v>
+        <f>A16/A8</f>
+        <v>102.4</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>51.1875</v>
+        <f t="shared" si="0"/>
+        <v>51.2</v>
       </c>
       <c r="D8">
-        <f t="shared" si="2"/>
-        <v>204.75</v>
+        <f t="shared" si="1"/>
+        <v>204.8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -844,16 +844,16 @@
         <v>48</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>85.3125</v>
+        <f>A16/A9</f>
+        <v>85.333333333333329</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
-        <v>42.65625</v>
+        <f t="shared" si="0"/>
+        <v>42.666666666666664</v>
       </c>
       <c r="D9">
-        <f t="shared" si="2"/>
-        <v>170.625</v>
+        <f t="shared" si="1"/>
+        <v>170.66666666666666</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
@@ -861,16 +861,16 @@
         <v>60</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>68.25</v>
+        <f>A16/A10</f>
+        <v>68.266666666666666</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
-        <v>34.125</v>
+        <f t="shared" si="0"/>
+        <v>34.133333333333333</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
-        <v>136.5</v>
+        <f t="shared" si="1"/>
+        <v>136.53333333333333</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -878,25 +878,76 @@
         <v>80</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>51.1875</v>
+        <f>A16/A11</f>
+        <v>51.2</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
-        <v>25.59375</v>
+        <f t="shared" si="0"/>
+        <v>25.6</v>
       </c>
       <c r="D11">
+        <f t="shared" si="1"/>
+        <v>102.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>82</v>
+      </c>
+      <c r="B12">
+        <f>A16/A12</f>
+        <v>49.951219512195124</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C13" si="2">B12/2</f>
+        <v>24.975609756097562</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D13" si="3">B12*2</f>
+        <v>99.902439024390247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>83</v>
+      </c>
+      <c r="B13">
+        <f>A16/A13</f>
+        <v>49.349397590361448</v>
+      </c>
+      <c r="C13">
         <f t="shared" si="2"/>
-        <v>102.375</v>
+        <v>24.674698795180724</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="3"/>
+        <v>98.698795180722897</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
-        <v>4095</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18">
+        <v>88</v>
+      </c>
+      <c r="B14">
+        <f>A16/A14</f>
+        <v>46.545454545454547</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14" si="4">B14/2</f>
+        <v>23.272727272727273</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14" si="5">B14*2</f>
+        <v>93.090909090909093</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20">
         <f>SUM(A4:A10)</f>
         <v>232</v>
       </c>

</xml_diff>